<commit_message>
big update. identifier works
</commit_message>
<xml_diff>
--- a/src/main/resources/importfiles/testfiles/Preisanfrage Sonepar.xlsx
+++ b/src/main/resources/importfiles/testfiles/Preisanfrage Sonepar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F01D3F-8503-4330-9690-5CADCFC3AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32340EB7-93E7-41CA-9EFE-1CC35B39B10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A47D82A6-F454-4081-97EF-3A1C601899E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Kundenartikel-
 nummer</t>
@@ -76,6 +76,12 @@
     <t>NR.22</t>
   </si>
   <si>
+    <t>SCOTCHBAND SUPER 88 19X20M SW</t>
+  </si>
+  <si>
+    <t>SUPER 88</t>
+  </si>
+  <si>
     <t>FI-SCHALTER</t>
   </si>
   <si>
@@ -98,6 +104,15 @@
   </si>
   <si>
     <t>2CKA001725A0548</t>
+  </si>
+  <si>
+    <t>AP FR TASTER SCHLIESSER</t>
+  </si>
+  <si>
+    <t>2621 W-53</t>
+  </si>
+  <si>
+    <t>2CKA001484A0370</t>
   </si>
   <si>
     <t>DEHN</t>
@@ -229,12 +244,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -352,8 +373,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -372,25 +412,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,6 +431,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -725,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4E67BB-9B27-4779-A0B1-C4E454E76F52}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,67 +787,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="16">
         <v>7000042539</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="17">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12">
+      <c r="H2" s="18"/>
+      <c r="I2" s="19">
         <v>48</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="20">
         <f t="shared" ref="J2:J5" si="0">H2/F2*I2</f>
         <v>0</v>
       </c>
@@ -815,32 +856,32 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="A3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10">
+      <c r="D3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="17">
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12">
+      <c r="H3" s="18"/>
+      <c r="I3" s="19">
         <v>3</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -849,32 +890,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="F4" s="17">
         <v>1</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19">
         <v>11</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -883,32 +924,32 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="A5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="15">
         <v>318033</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="16">
         <v>318033</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="E5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="17">
         <v>1</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19">
         <v>100</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -917,33 +958,33 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="17">
+      <c r="A6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="24">
         <v>100</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19">
+      <c r="H6" s="25"/>
+      <c r="I6" s="26">
         <v>20</v>
       </c>
-      <c r="J6" s="20">
-        <f t="shared" ref="J6:J7" si="1">H6/F6*I6</f>
+      <c r="J6" s="27">
+        <f t="shared" ref="J6:J8" si="1">H6/F6*I6</f>
         <v>0</v>
       </c>
       <c r="K6">
@@ -951,71 +992,134 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="9">
-        <v>4008321873743</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="A7" s="6">
+        <v>10232</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12">
-        <v>5</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="H7" s="5"/>
+      <c r="I7" s="4">
+        <v>25</v>
+      </c>
+      <c r="J7" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>120340313</v>
-      </c>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="A8" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="16">
+        <v>4008321873743</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19">
+        <v>5</v>
+      </c>
+      <c r="J8" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>120340313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="17">
         <v>100</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12">
+      <c r="H9" s="18"/>
+      <c r="I9" s="19">
         <v>100</v>
       </c>
-      <c r="J8" s="13">
-        <f t="shared" ref="J8" si="2">H8/F8*I8</f>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9:J10" si="2">H9/F9*I9</f>
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <v>120119722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15527</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>7100079942</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4">
+        <v>50</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>